<commit_message>
adding the updated BOMs
</commit_message>
<xml_diff>
--- a/BOMs/Controller.xlsx
+++ b/BOMs/Controller.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akash\Desktop\UIUCClasses\ECE445\SeniorDesign\BOMs\Final_BOMs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akash\Desktop\UIUCClasses\ECE445\SeniorDesign\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECE2C89-31FE-4DE5-AC11-BA6BBC3D8620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A39FBD-9741-47F1-B678-761450FE3D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4508DFA6-70BC-40B5-BE46-A6E4381AF8BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="145">
   <si>
     <t>Comment</t>
   </si>
@@ -212,9 +212,6 @@
     <t>744235900</t>
   </si>
   <si>
-    <t>Data Line Filter, 2 Function(s), 60V, 2A, 4 Pin(s)</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -437,9 +434,6 @@
     <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74LV4T125PWR/4806529</t>
   </si>
   <si>
-    <t>PSN74LV4T125QPWRQ1*</t>
-  </si>
-  <si>
     <t>REF2033QDDCRQ1*</t>
   </si>
   <si>
@@ -462,6 +456,24 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/infineon-technologies/2N7002H6327XTSA2/5410097</t>
+  </si>
+  <si>
+    <t>3.3V to 5V level shifter</t>
+  </si>
+  <si>
+    <t>5V LDO</t>
+  </si>
+  <si>
+    <t>CAN Choke</t>
+  </si>
+  <si>
+    <t>3.3V LDO</t>
+  </si>
+  <si>
+    <t>NMOS for the ALARM system</t>
+  </si>
+  <si>
+    <t>PSN74LV4T125QPWRQ1</t>
   </si>
 </sst>
 </file>
@@ -495,7 +507,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,6 +517,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,7 +556,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -554,6 +572,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -892,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DFB67A-128C-479E-8520-956AD6629EB7}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,13 +943,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
@@ -948,7 +972,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5">
@@ -976,7 +1000,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5">
@@ -1004,7 +1028,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5">
@@ -1032,7 +1056,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5">
@@ -1060,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5">
@@ -1088,7 +1112,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5">
@@ -1116,7 +1140,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5">
@@ -1144,7 +1168,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5">
@@ -1166,13 +1190,13 @@
         <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E10" s="5">
         <v>0.37</v>
@@ -1196,13 +1220,13 @@
         <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E11" s="5">
         <v>0.15</v>
@@ -1226,13 +1250,13 @@
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="1">
         <v>8</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E12" s="5">
         <v>0.15</v>
@@ -1262,7 +1286,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E13" s="5">
         <v>3.81</v>
@@ -1292,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5">
@@ -1320,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5">
@@ -1348,7 +1372,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E16" s="5">
         <v>1.95</v>
@@ -1372,13 +1396,13 @@
         <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E17" s="5">
         <v>1.8</v>
@@ -1388,27 +1412,27 @@
         <v>1.8</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E18" s="5">
         <v>0.4</v>
@@ -1418,27 +1442,27 @@
         <v>0.4</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>143</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E19" s="5">
         <v>0.32</v>
@@ -1448,27 +1472,27 @@
         <v>0.32</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C20" s="1">
         <v>21</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5">
@@ -1476,13 +1500,13 @@
         <v>0</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1490,13 +1514,13 @@
         <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1">
         <v>15</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5">
@@ -1504,18 +1528,18 @@
         <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>25</v>
@@ -1524,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5">
@@ -1532,18 +1556,18 @@
         <v>0</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
@@ -1552,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5">
@@ -1560,18 +1584,18 @@
         <v>0</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>25</v>
@@ -1580,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5">
@@ -1588,18 +1612,18 @@
         <v>0</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>25</v>
@@ -1608,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5">
@@ -1616,27 +1640,27 @@
         <v>0</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E26" s="5">
         <v>1.87</v>
@@ -1646,27 +1670,27 @@
         <v>3.74</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E27" s="5">
         <v>1.64</v>
@@ -1676,18 +1700,18 @@
         <v>1.64</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="I27" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>25</v>
@@ -1696,7 +1720,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5">
@@ -1704,57 +1728,57 @@
         <v>0</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="10">
+        <v>1</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="12">
+        <v>3.69</v>
+      </c>
+      <c r="F29" s="12">
+        <f t="shared" si="0"/>
+        <v>3.69</v>
+      </c>
+      <c r="G29" s="9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E29" s="5">
-        <v>3.69</v>
-      </c>
-      <c r="F29" s="5">
-        <f t="shared" si="0"/>
-        <v>3.69</v>
-      </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E30" s="5">
         <v>1</v>
@@ -1764,27 +1788,27 @@
         <v>2</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5">
@@ -1792,27 +1816,27 @@
         <v>0</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E32" s="5">
         <v>0.86</v>
@@ -1822,13 +1846,13 @@
         <v>0.86</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed orders, updated notebook
</commit_message>
<xml_diff>
--- a/BOMs/Controller.xlsx
+++ b/BOMs/Controller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhruv\Documents\College\ECE\445\SeniorDesign\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6129477-197D-48D2-85F1-23342DAC359D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A485F7B-7BB8-4F88-B2BD-6F61A815DE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{4508DFA6-70BC-40B5-BE46-A6E4381AF8BA}"/>
   </bookViews>
@@ -551,7 +551,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -562,9 +562,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
@@ -919,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DFB67A-128C-479E-8520-956AD6629EB7}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1188,123 +1185,123 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>1</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>0.37</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="16">
         <f t="shared" si="0"/>
         <v>0.37</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>4</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="16">
         <v>0.15</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="16">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>8</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>0.15</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>4</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <v>3.81</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="16">
         <f t="shared" si="0"/>
         <v>15.24</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="13" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1364,123 +1361,123 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A16" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="14">
         <v>1</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="16">
         <v>1.95</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="16">
         <f t="shared" si="0"/>
         <v>1.95</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <v>1</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="16">
         <v>1.8</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="16">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <v>1</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="16">
         <v>0.4</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="16">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <v>1</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="16">
         <v>0.32</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="16">
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="13" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1652,63 +1649,63 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <v>2</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="16">
         <v>1.87</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="16">
         <f t="shared" si="0"/>
         <v>3.74</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:9" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A27" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="14">
         <v>1</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="16">
         <v>1.64</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="16">
         <f t="shared" si="0"/>
         <v>1.64</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="13" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1741,62 +1738,62 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="9">
         <v>1</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="11">
         <v>3.69</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="11">
         <f t="shared" si="0"/>
         <v>3.69</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="H29" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="14" t="s">
+    <row r="30" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="14">
         <v>2</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="16">
         <v>1</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="13" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1828,38 +1825,38 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:9" s="17" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A32" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="14">
         <v>1</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="16">
         <v>0.86</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="16">
         <f t="shared" si="0"/>
         <v>0.86</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="13" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.45">
-      <c r="F33" s="13">
+      <c r="F33" s="12">
         <f>SUM(F2:F32)</f>
         <v>33.81</v>
       </c>

</xml_diff>